<commit_message>
Completed creating a formula without validation, Add validation on bars and mandrel constraints
</commit_message>
<xml_diff>
--- a/Docs/CS297_TimeTracking.xlsx
+++ b/Docs/CS297_TimeTracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\Lane Stuff\CS297\CapstoneMasons\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\CapstoneMasons\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D6D511-2F6D-4A4F-943F-BC56921176F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E49681-2751-43F2-8CCF-936576A5C195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="735" windowWidth="27150" windowHeight="17790" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Totals" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Week 9" sheetId="12" r:id="rId10"/>
     <sheet name="Week 10" sheetId="13" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,9 +33,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -46,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="29">
   <si>
     <t>Week 1</t>
   </si>
@@ -130,6 +128,9 @@
   </si>
   <si>
     <t>Masons Supply</t>
+  </si>
+  <si>
+    <t>Dane Woods</t>
   </si>
 </sst>
 </file>
@@ -458,9 +459,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -468,7 +469,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -485,7 +486,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -511,7 +512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -541,14 +542,14 @@
       </c>
       <c r="H4">
         <f>'Week 1'!I$9</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I4">
         <f>H4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -582,10 +583,10 @@
       </c>
       <c r="I5">
         <f>H5+I4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -619,10 +620,10 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -656,10 +657,10 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -693,10 +694,10 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -730,10 +731,10 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -767,10 +768,10 @@
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -804,10 +805,10 @@
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -841,10 +842,10 @@
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -878,15 +879,15 @@
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -905,9 +906,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -916,7 +917,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -937,7 +938,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -963,7 +964,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -988,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1013,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1038,7 +1039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1063,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1088,7 +1089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1113,7 +1114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1133,9 +1134,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1144,7 +1145,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1165,7 +1166,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1191,7 +1192,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1216,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1241,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1266,7 +1267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1291,7 +1292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1316,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1341,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1358,12 +1359,12 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1372,7 +1373,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1388,12 +1389,11 @@
         <f>Totals!F2</f>
         <v>Name 3</v>
       </c>
-      <c r="H2" t="str">
-        <f>Totals!H2</f>
-        <v>Name 4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1440,13 +1440,15 @@
         <f>F4</f>
         <v>0</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1">
+        <v>2</v>
+      </c>
       <c r="I4">
         <f>H4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1467,13 +1469,15 @@
         <f>F5+G4</f>
         <v>0</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1">
+        <v>2</v>
+      </c>
       <c r="I5">
         <f>H5+I4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1492,13 +1496,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1520,10 +1526,10 @@
       <c r="H7" s="1"/>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1545,10 +1551,10 @@
       <c r="H8" s="1"/>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1570,10 +1576,10 @@
       <c r="H9" s="1"/>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1593,9 +1599,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1604,7 +1610,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1625,7 +1631,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1651,7 +1657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1676,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1701,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1726,7 +1732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1751,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1776,7 +1782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1801,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1821,9 +1827,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1832,7 +1838,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1853,7 +1859,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1879,7 +1885,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1904,7 +1910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1929,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1954,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1979,7 +1985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2004,7 +2010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2029,7 +2035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2049,9 +2055,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2060,7 +2066,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2081,7 +2087,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -2107,7 +2113,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2132,7 +2138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2157,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2182,7 +2188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2207,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2232,7 +2238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2257,7 +2263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2277,9 +2283,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2288,7 +2294,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2309,7 +2315,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -2335,7 +2341,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2360,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2385,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2410,7 +2416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2435,7 +2441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2460,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2485,7 +2491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2505,9 +2511,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2516,7 +2522,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2537,7 +2543,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -2563,7 +2569,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2588,7 +2594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2613,7 +2619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2638,7 +2644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2663,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2688,7 +2694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2713,7 +2719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2733,9 +2739,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2744,7 +2750,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2765,7 +2771,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -2791,7 +2797,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2816,7 +2822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2841,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2866,7 +2872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2891,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2916,7 +2922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2941,7 +2947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2961,9 +2967,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2972,7 +2978,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2993,7 +2999,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -3019,7 +3025,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3044,7 +3050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -3069,7 +3075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -3094,7 +3100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -3119,7 +3125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -3144,7 +3150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -3169,7 +3175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Added unit tests, comments to methods, and Team Contact to Docs
</commit_message>
<xml_diff>
--- a/Docs/CS297_TimeTracking.xlsx
+++ b/Docs/CS297_TimeTracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\CapstoneMasons\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\Lane Stuff\CS297\CapstoneMasons\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E49681-2751-43F2-8CCF-936576A5C195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB2B71F-4721-45F5-A6D3-318FDDD00489}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="735" windowWidth="27150" windowHeight="17790" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Totals" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Week 9" sheetId="12" r:id="rId10"/>
     <sheet name="Week 10" sheetId="13" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,7 +33,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -459,9 +461,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -469,7 +471,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -486,7 +488,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -512,17 +514,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4">
         <f>'Week 1'!C$9</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <f>B4</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <f>'Week 1'!E$9</f>
@@ -549,7 +551,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -559,7 +561,7 @@
       </c>
       <c r="C5">
         <f>B5+C4</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <f>'Week 2'!E$9</f>
@@ -586,7 +588,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -596,7 +598,7 @@
       </c>
       <c r="C6">
         <f t="shared" ref="C6:I13" si="0">B6+C5</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <f>'Week 3'!E$9</f>
@@ -623,7 +625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -633,7 +635,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <f>'Week 4'!E$9</f>
@@ -660,7 +662,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -670,7 +672,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <f>'Week 5'!E$9</f>
@@ -697,7 +699,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -707,7 +709,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <f>'Week 6'!E$9</f>
@@ -734,7 +736,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -744,7 +746,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <f>'Week 7'!E$9</f>
@@ -771,7 +773,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -781,7 +783,7 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <f>'Week 8'!E$9</f>
@@ -808,7 +810,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -818,7 +820,7 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <f>'Week 9'!E$9</f>
@@ -845,7 +847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -855,7 +857,7 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <f>'Week 10'!E$9</f>
@@ -882,12 +884,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -906,9 +908,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -917,7 +919,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -938,7 +940,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -964,7 +966,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -989,7 +991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1014,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1039,7 +1041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1064,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1089,7 +1091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1114,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1134,9 +1136,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1145,7 +1147,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1166,7 +1168,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1192,7 +1194,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1217,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1242,7 +1244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1267,7 +1269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1292,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1317,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1342,7 +1344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1359,12 +1361,12 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1373,7 +1375,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1393,7 +1395,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1419,7 +1421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1448,7 +1450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1477,14 +1479,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
       <c r="C6">
         <f t="shared" ref="C6:I9" si="0">B6+C5</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6">
@@ -1504,14 +1508,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7">
@@ -1529,14 +1533,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8">
@@ -1554,14 +1558,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9">
@@ -1579,7 +1583,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1599,9 +1603,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1610,7 +1614,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1631,7 +1635,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1657,7 +1661,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1682,7 +1686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1707,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1732,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1757,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1782,7 +1786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1807,7 +1811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1827,9 +1831,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1838,7 +1842,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1859,7 +1863,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1885,7 +1889,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1910,7 +1914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1935,7 +1939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1960,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1985,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2010,7 +2014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2035,7 +2039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2055,9 +2059,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2066,7 +2070,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2087,7 +2091,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -2113,7 +2117,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2138,7 +2142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2163,7 +2167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2188,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2213,7 +2217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2238,7 +2242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2263,7 +2267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2283,9 +2287,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2294,7 +2298,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2315,7 +2319,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -2341,7 +2345,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2366,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2391,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2416,7 +2420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2441,7 +2445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2466,7 +2470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2491,7 +2495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2511,9 +2515,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2522,7 +2526,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2543,7 +2547,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -2569,7 +2573,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2594,7 +2598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2619,7 +2623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2644,7 +2648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2669,7 +2673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2694,7 +2698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2719,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2739,9 +2743,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2750,7 +2754,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2771,7 +2775,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -2797,7 +2801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2822,7 +2826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2847,7 +2851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2872,7 +2876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2897,7 +2901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2922,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2947,7 +2951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2967,9 +2971,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2978,7 +2982,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2999,7 +3003,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -3025,7 +3029,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3050,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -3075,7 +3079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -3100,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -3125,7 +3129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -3150,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -3175,7 +3179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
People need to update their hours
</commit_message>
<xml_diff>
--- a/Docs/CS297_TimeTracking.xlsx
+++ b/Docs/CS297_TimeTracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\Lane Stuff\CS297\CapstoneMasons\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\CS297\CapstoneMasons\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB2B71F-4721-45F5-A6D3-318FDDD00489}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DDEF01-7C5B-4C62-973C-12DDA9586FCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="735" windowWidth="27150" windowHeight="17790" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Totals" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Week 9" sheetId="12" r:id="rId10"/>
     <sheet name="Week 10" sheetId="13" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,9 +33,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -46,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="32">
   <si>
     <t>Week 1</t>
   </si>
@@ -133,6 +131,15 @@
   </si>
   <si>
     <t>Dane Woods</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Jeff Walters</t>
+  </si>
+  <si>
+    <t>Gino Betetta</t>
   </si>
 </sst>
 </file>
@@ -461,9 +468,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -471,7 +478,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -488,7 +495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -514,44 +521,44 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4">
-        <f>'Week 1'!C$9</f>
-        <v>8</v>
+        <f>'Week 1'!C$10</f>
+        <v>11</v>
       </c>
       <c r="C4">
         <f>B4</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D4">
-        <f>'Week 1'!E$9</f>
-        <v>0</v>
+        <f>'Week 1'!E$10</f>
+        <v>13</v>
       </c>
       <c r="E4">
         <f>D4</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F4">
-        <f>'Week 1'!G$9</f>
-        <v>0</v>
+        <f>'Week 1'!G$10</f>
+        <v>10</v>
       </c>
       <c r="G4">
         <f>F4</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H4">
-        <f>'Week 1'!I$9</f>
-        <v>8</v>
+        <f>'Week 1'!I$10</f>
+        <v>14</v>
       </c>
       <c r="I4">
         <f>H4</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -561,7 +568,7 @@
       </c>
       <c r="C5">
         <f>B5+C4</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <f>'Week 2'!E$9</f>
@@ -569,7 +576,7 @@
       </c>
       <c r="E5">
         <f>D5+E4</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F5">
         <f>'Week 2'!G$9</f>
@@ -577,7 +584,7 @@
       </c>
       <c r="G5">
         <f>F5+G4</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H5">
         <f>'Week 2'!I$9</f>
@@ -585,10 +592,10 @@
       </c>
       <c r="I5">
         <f>H5+I4</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -598,7 +605,7 @@
       </c>
       <c r="C6">
         <f t="shared" ref="C6:I13" si="0">B6+C5</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <f>'Week 3'!E$9</f>
@@ -606,7 +613,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F6">
         <f>'Week 3'!G$9</f>
@@ -614,7 +621,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H6">
         <f>'Week 3'!I$9</f>
@@ -622,10 +629,10 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -635,7 +642,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <f>'Week 4'!E$9</f>
@@ -643,7 +650,7 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F7">
         <f>'Week 4'!G$9</f>
@@ -651,7 +658,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H7">
         <f>'Week 4'!I$9</f>
@@ -659,10 +666,10 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -672,7 +679,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <f>'Week 5'!E$9</f>
@@ -680,7 +687,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F8">
         <f>'Week 5'!G$9</f>
@@ -688,7 +695,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H8">
         <f>'Week 5'!I$9</f>
@@ -696,10 +703,10 @@
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -709,7 +716,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <f>'Week 6'!E$9</f>
@@ -717,7 +724,7 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F9">
         <f>'Week 6'!G$9</f>
@@ -725,7 +732,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H9">
         <f>'Week 6'!I$9</f>
@@ -733,10 +740,10 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -746,7 +753,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <f>'Week 7'!E$9</f>
@@ -754,7 +761,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F10">
         <f>'Week 7'!G$9</f>
@@ -762,7 +769,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H10">
         <f>'Week 7'!I$9</f>
@@ -770,10 +777,10 @@
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -783,7 +790,7 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D11">
         <f>'Week 8'!E$9</f>
@@ -791,7 +798,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F11">
         <f>'Week 8'!G$9</f>
@@ -799,7 +806,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H11">
         <f>'Week 8'!I$9</f>
@@ -807,10 +814,10 @@
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -820,7 +827,7 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D12">
         <f>'Week 9'!E$9</f>
@@ -828,7 +835,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F12">
         <f>'Week 9'!G$9</f>
@@ -836,7 +843,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H12">
         <f>'Week 9'!I$9</f>
@@ -844,10 +851,10 @@
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -857,7 +864,7 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D13">
         <f>'Week 10'!E$9</f>
@@ -865,7 +872,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F13">
         <f>'Week 10'!G$9</f>
@@ -873,7 +880,7 @@
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H13">
         <f>'Week 10'!I$9</f>
@@ -881,15 +888,15 @@
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -908,9 +915,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -919,7 +926,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -940,7 +947,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -966,7 +973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -991,7 +998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1016,7 +1023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1041,7 +1048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1066,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1091,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1116,7 +1123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1136,9 +1143,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1147,7 +1154,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1168,7 +1175,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1194,7 +1201,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1219,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1244,7 +1251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1269,7 +1276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1294,7 +1301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1319,7 +1326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1344,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1358,15 +1365,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC11E001-DA2D-DB40-B076-5732B774C833}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1375,7 +1382,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1383,19 +1390,17 @@
         <f>Totals!B2</f>
         <v>Jacob Felten</v>
       </c>
-      <c r="D2" t="str">
-        <f>Totals!D2</f>
-        <v>Name 2</v>
-      </c>
-      <c r="F2" t="str">
-        <f>Totals!F2</f>
-        <v>Name 3</v>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
       </c>
       <c r="H2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1421,7 +1426,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1432,15 +1437,19 @@
         <f>B4</f>
         <v>2</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
       <c r="E4">
         <f>D4</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
       <c r="G4">
         <f>F4</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H4" s="1">
         <v>2</v>
@@ -1450,7 +1459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1461,15 +1470,19 @@
         <f>B5+C4</f>
         <v>6</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
       <c r="E5">
         <f>D5+E4</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
       <c r="G5">
         <f>F5+G4</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H5" s="1">
         <v>2</v>
@@ -1479,112 +1492,157 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:I9" si="0">B6+C5</f>
+        <f>B6+C5</f>
         <v>8</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="1"/>
+        <f>D6+E5</f>
+        <v>7</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
       <c r="G6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>F6+G5</f>
+        <v>8</v>
       </c>
       <c r="H6" s="1">
         <v>4</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f>H6+I5</f>
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <f>B7+C6</f>
+        <v>11</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <f>D7+E6</f>
+        <v>9</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <f>F7+G6</f>
+        <v>10</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <f>H7+I6</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>20</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="D8" s="1"/>
+        <f t="shared" ref="C8:I10" si="0">B8+C7</f>
+        <v>11</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2</v>
+      </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1603,9 +1661,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1614,7 +1672,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1635,7 +1693,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1661,7 +1719,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1686,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1711,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1736,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1761,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1786,7 +1844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1811,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1831,9 +1889,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1842,7 +1900,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1863,7 +1921,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1889,7 +1947,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1914,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1939,7 +1997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1964,7 +2022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1989,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2014,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2039,7 +2097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2059,9 +2117,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2070,7 +2128,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2091,7 +2149,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -2117,7 +2175,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2142,7 +2200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2167,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2192,7 +2250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2217,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2242,7 +2300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2267,7 +2325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2287,9 +2345,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2298,7 +2356,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2319,7 +2377,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -2345,7 +2403,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2370,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2395,7 +2453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2420,7 +2478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2445,7 +2503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2470,7 +2528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2495,7 +2553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2515,9 +2573,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2526,7 +2584,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2547,7 +2605,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -2573,7 +2631,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2598,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2623,7 +2681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2648,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2673,7 +2731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2698,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2723,7 +2781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2743,9 +2801,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2754,7 +2812,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2775,7 +2833,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -2801,7 +2859,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2826,7 +2884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2851,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2876,7 +2934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2901,7 +2959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2926,7 +2984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2951,7 +3009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2971,9 +3029,9 @@
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2982,7 +3040,7 @@
         <v>Masons Supply</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -3003,7 +3061,7 @@
         <v>Name 4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -3029,7 +3087,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -3054,7 +3112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -3079,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -3104,7 +3162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -3129,7 +3187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -3154,7 +3212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -3179,7 +3237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Gino and Jacob need to update hours
</commit_message>
<xml_diff>
--- a/Docs/CS297_TimeTracking.xlsx
+++ b/Docs/CS297_TimeTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\CS297\CapstoneMasons\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DDEF01-7C5B-4C62-973C-12DDA9586FCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12993648-89CC-4BF9-A028-7120E677F392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4830" yWindow="735" windowWidth="27150" windowHeight="17790" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="29">
   <si>
     <t>Week 1</t>
   </si>
@@ -74,15 +74,6 @@
   </si>
   <si>
     <t>Week 10</t>
-  </si>
-  <si>
-    <t>Name 2</t>
-  </si>
-  <si>
-    <t>Name 3</t>
-  </si>
-  <si>
-    <t>Name 4</t>
   </si>
   <si>
     <t>Total</t>
@@ -465,60 +456,60 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -893,12 +884,12 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -919,7 +910,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="str">
         <f>Totals!B1</f>
@@ -928,7 +919,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" t="str">
         <f>Totals!B2</f>
@@ -936,46 +927,46 @@
       </c>
       <c r="D2" t="str">
         <f>Totals!D2</f>
-        <v>Name 2</v>
+        <v>Jeff Walters</v>
       </c>
       <c r="F2" t="str">
         <f>Totals!F2</f>
-        <v>Name 3</v>
+        <v>Gino Betetta</v>
       </c>
       <c r="H2" t="str">
         <f>Totals!H2</f>
-        <v>Name 4</v>
+        <v>Dane Woods</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4">
@@ -1000,7 +991,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5">
@@ -1025,7 +1016,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
@@ -1050,7 +1041,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
@@ -1075,7 +1066,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
@@ -1100,7 +1091,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -1125,7 +1116,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1147,7 +1138,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="str">
         <f>Totals!B1</f>
@@ -1156,7 +1147,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" t="str">
         <f>Totals!B2</f>
@@ -1164,46 +1155,46 @@
       </c>
       <c r="D2" t="str">
         <f>Totals!D2</f>
-        <v>Name 2</v>
+        <v>Jeff Walters</v>
       </c>
       <c r="F2" t="str">
         <f>Totals!F2</f>
-        <v>Name 3</v>
+        <v>Gino Betetta</v>
       </c>
       <c r="H2" t="str">
         <f>Totals!H2</f>
-        <v>Name 4</v>
+        <v>Dane Woods</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4">
@@ -1228,7 +1219,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5">
@@ -1253,7 +1244,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
@@ -1278,7 +1269,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
@@ -1303,7 +1294,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
@@ -1328,7 +1319,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -1353,7 +1344,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1368,14 +1359,14 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="str">
         <f>Totals!B1</f>
@@ -1384,51 +1375,51 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" t="str">
         <f>Totals!B2</f>
         <v>Jacob Felten</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -1461,7 +1452,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -1494,7 +1485,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -1527,7 +1518,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
@@ -1560,7 +1551,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
@@ -1589,14 +1580,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
       <c r="E9">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1616,14 +1609,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
       <c r="E10">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1643,7 +1638,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1665,7 +1660,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="str">
         <f>Totals!B1</f>
@@ -1674,7 +1669,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" t="str">
         <f>Totals!B2</f>
@@ -1682,46 +1677,46 @@
       </c>
       <c r="D2" t="str">
         <f>Totals!D2</f>
-        <v>Name 2</v>
+        <v>Jeff Walters</v>
       </c>
       <c r="F2" t="str">
         <f>Totals!F2</f>
-        <v>Name 3</v>
+        <v>Gino Betetta</v>
       </c>
       <c r="H2" t="str">
         <f>Totals!H2</f>
-        <v>Name 4</v>
+        <v>Dane Woods</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4">
@@ -1746,7 +1741,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5">
@@ -1771,7 +1766,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
@@ -1796,7 +1791,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
@@ -1821,7 +1816,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
@@ -1846,7 +1841,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -1871,7 +1866,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1893,7 +1888,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="str">
         <f>Totals!B1</f>
@@ -1902,7 +1897,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" t="str">
         <f>Totals!B2</f>
@@ -1910,46 +1905,46 @@
       </c>
       <c r="D2" t="str">
         <f>Totals!D2</f>
-        <v>Name 2</v>
+        <v>Jeff Walters</v>
       </c>
       <c r="F2" t="str">
         <f>Totals!F2</f>
-        <v>Name 3</v>
+        <v>Gino Betetta</v>
       </c>
       <c r="H2" t="str">
         <f>Totals!H2</f>
-        <v>Name 4</v>
+        <v>Dane Woods</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4">
@@ -1974,7 +1969,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5">
@@ -1999,7 +1994,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
@@ -2024,7 +2019,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
@@ -2049,7 +2044,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
@@ -2074,7 +2069,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -2099,7 +2094,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2121,7 +2116,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="str">
         <f>Totals!B1</f>
@@ -2130,7 +2125,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" t="str">
         <f>Totals!B2</f>
@@ -2138,46 +2133,46 @@
       </c>
       <c r="D2" t="str">
         <f>Totals!D2</f>
-        <v>Name 2</v>
+        <v>Jeff Walters</v>
       </c>
       <c r="F2" t="str">
         <f>Totals!F2</f>
-        <v>Name 3</v>
+        <v>Gino Betetta</v>
       </c>
       <c r="H2" t="str">
         <f>Totals!H2</f>
-        <v>Name 4</v>
+        <v>Dane Woods</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4">
@@ -2202,7 +2197,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5">
@@ -2227,7 +2222,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
@@ -2252,7 +2247,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
@@ -2277,7 +2272,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
@@ -2302,7 +2297,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -2327,7 +2322,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2349,7 +2344,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="str">
         <f>Totals!B1</f>
@@ -2358,7 +2353,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" t="str">
         <f>Totals!B2</f>
@@ -2366,46 +2361,46 @@
       </c>
       <c r="D2" t="str">
         <f>Totals!D2</f>
-        <v>Name 2</v>
+        <v>Jeff Walters</v>
       </c>
       <c r="F2" t="str">
         <f>Totals!F2</f>
-        <v>Name 3</v>
+        <v>Gino Betetta</v>
       </c>
       <c r="H2" t="str">
         <f>Totals!H2</f>
-        <v>Name 4</v>
+        <v>Dane Woods</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4">
@@ -2430,7 +2425,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5">
@@ -2455,7 +2450,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
@@ -2480,7 +2475,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
@@ -2505,7 +2500,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
@@ -2530,7 +2525,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -2555,7 +2550,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2577,7 +2572,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="str">
         <f>Totals!B1</f>
@@ -2586,7 +2581,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" t="str">
         <f>Totals!B2</f>
@@ -2594,46 +2589,46 @@
       </c>
       <c r="D2" t="str">
         <f>Totals!D2</f>
-        <v>Name 2</v>
+        <v>Jeff Walters</v>
       </c>
       <c r="F2" t="str">
         <f>Totals!F2</f>
-        <v>Name 3</v>
+        <v>Gino Betetta</v>
       </c>
       <c r="H2" t="str">
         <f>Totals!H2</f>
-        <v>Name 4</v>
+        <v>Dane Woods</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4">
@@ -2658,7 +2653,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5">
@@ -2683,7 +2678,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
@@ -2708,7 +2703,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
@@ -2733,7 +2728,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
@@ -2758,7 +2753,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -2783,7 +2778,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2805,7 +2800,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="str">
         <f>Totals!B1</f>
@@ -2814,7 +2809,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" t="str">
         <f>Totals!B2</f>
@@ -2822,46 +2817,46 @@
       </c>
       <c r="D2" t="str">
         <f>Totals!D2</f>
-        <v>Name 2</v>
+        <v>Jeff Walters</v>
       </c>
       <c r="F2" t="str">
         <f>Totals!F2</f>
-        <v>Name 3</v>
+        <v>Gino Betetta</v>
       </c>
       <c r="H2" t="str">
         <f>Totals!H2</f>
-        <v>Name 4</v>
+        <v>Dane Woods</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4">
@@ -2886,7 +2881,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5">
@@ -2911,7 +2906,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
@@ -2936,7 +2931,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
@@ -2961,7 +2956,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
@@ -2986,7 +2981,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -3011,7 +3006,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3033,7 +3028,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="str">
         <f>Totals!B1</f>
@@ -3042,7 +3037,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" t="str">
         <f>Totals!B2</f>
@@ -3050,46 +3045,46 @@
       </c>
       <c r="D2" t="str">
         <f>Totals!D2</f>
-        <v>Name 2</v>
+        <v>Jeff Walters</v>
       </c>
       <c r="F2" t="str">
         <f>Totals!F2</f>
-        <v>Name 3</v>
+        <v>Gino Betetta</v>
       </c>
       <c r="H2" t="str">
         <f>Totals!H2</f>
-        <v>Name 4</v>
+        <v>Dane Woods</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4">
@@ -3114,7 +3109,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5">
@@ -3139,7 +3134,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
@@ -3164,7 +3159,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
@@ -3189,7 +3184,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
@@ -3214,7 +3209,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
@@ -3239,7 +3234,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>